<commit_message>
Refactored map class in order to fit other modules #AB113
</commit_message>
<xml_diff>
--- a/resources/base_table.xlsx
+++ b/resources/base_table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\6sem\proj\Shopping-Mall-Maps\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\study\6sem\proj\blank\Shopping-Mall-Maps\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B36F4D12-9EC1-4810-8F15-341A191B998F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9E04EC-8D77-4E4E-804A-E3A3C42463D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{50C593A5-B430-4920-BCA3-890D689CD91B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>true</t>
   </si>
@@ -78,18 +78,6 @@
 The best shop ever!</t>
   </si>
   <si>
-    <t>shop1_1</t>
-  </si>
-  <si>
-    <t>shop1_2</t>
-  </si>
-  <si>
-    <t>fancy diamond shop!</t>
-  </si>
-  <si>
-    <t>poor rectangle</t>
-  </si>
-  <si>
     <t>I've made it look like a description</t>
   </si>
   <si>
@@ -118,13 +106,97 @@
   </si>
   <si>
     <t>full_info</t>
+  </si>
+  <si>
+    <t>1_shop_6</t>
+  </si>
+  <si>
+    <t>1_shop_4</t>
+  </si>
+  <si>
+    <t>1_shop_3</t>
+  </si>
+  <si>
+    <t>1_shop_2</t>
+  </si>
+  <si>
+    <t>1_shop_1</t>
+  </si>
+  <si>
+    <t>2_shop_4</t>
+  </si>
+  <si>
+    <t>2_shop_101</t>
+  </si>
+  <si>
+    <t>2_shop_104</t>
+  </si>
+  <si>
+    <t>2_shop_103</t>
+  </si>
+  <si>
+    <t>2_shop_102</t>
+  </si>
+  <si>
+    <t>2_shop_5</t>
+  </si>
+  <si>
+    <t>3_shop_201</t>
+  </si>
+  <si>
+    <t>2_toilet_101</t>
+  </si>
+  <si>
+    <t>toilet</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>kitchen</t>
+  </si>
+  <si>
+    <t>Yakov's room</t>
+  </si>
+  <si>
+    <t>his brother's room</t>
+  </si>
+  <si>
+    <t>1_toilet_1</t>
+  </si>
+  <si>
+    <t>cabinet</t>
+  </si>
+  <si>
+    <t>bathroom</t>
+  </si>
+  <si>
+    <t>sophisticated shaped shop</t>
+  </si>
+  <si>
+    <t>bizarre filled shop</t>
+  </si>
+  <si>
+    <t>just a shop</t>
+  </si>
+  <si>
+    <t>another shop</t>
+  </si>
+  <si>
+    <t>and another shop</t>
+  </si>
+  <si>
+    <t>big shop</t>
+  </si>
+  <si>
+    <t>shop in the trees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +204,27 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,7 +235,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -150,27 +243,189 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFF0F0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FFF0F0F0"/>
+        </bottom>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -211,33 +466,33 @@
       </xs:element>
     </xs:schema>
   </Schema>
-  <Map ID="3" Name="Info_карта" RootElement="Info" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="3" Name="Info_карта" RootElement="Info" SchemaID="Schema3" ShowImportExportValidationErrors="true" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6DB9F9F4-29E5-4CFF-82B1-577E5665E995}" name="Таблица8" displayName="Таблица8" ref="A1:G3" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:G3" xr:uid="{C3EBD02F-7C3D-45D7-AC1A-107EC6888DC2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6DB9F9F4-29E5-4CFF-82B1-577E5665E995}" name="Таблица8" displayName="Таблица8" ref="A1:G15" tableType="xml" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:G15" xr:uid="{C3EBD02F-7C3D-45D7-AC1A-107EC6888DC2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{AC38BDA1-B3B8-40A4-969F-2B5589C7A1CC}" uniqueName="SVG_ID" name="SVG_ID">
+    <tableColumn id="1" xr3:uid="{AC38BDA1-B3B8-40A4-969F-2B5589C7A1CC}" uniqueName="SVG_ID" name="SVG_ID" dataDxfId="7">
       <xmlColumnPr mapId="3" xpath="/Info/InfoLine/SVG_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{AB7904E2-20DE-4B4F-87F0-FA0206D83421}" uniqueName="short_name" name="short_name">
+    <tableColumn id="2" xr3:uid="{AB7904E2-20DE-4B4F-87F0-FA0206D83421}" uniqueName="short_name" name="short_name" dataDxfId="6">
       <xmlColumnPr mapId="3" xpath="/Info/InfoLine/short_name" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6FE72EE9-A500-493B-8286-983B1BCB0807}" uniqueName="is_a_shop" name="is_a_shop">
+    <tableColumn id="3" xr3:uid="{6FE72EE9-A500-493B-8286-983B1BCB0807}" uniqueName="is_a_shop" name="is_a_shop" dataDxfId="5">
       <xmlColumnPr mapId="3" xpath="/Info/InfoLine/is_a_shop" xmlDataType="boolean"/>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0C6137E0-0FE7-41EC-886C-AB9003B28C14}" uniqueName="short_info" name="short_info">
+    <tableColumn id="4" xr3:uid="{0C6137E0-0FE7-41EC-886C-AB9003B28C14}" uniqueName="short_info" name="short_info" dataDxfId="4">
       <xmlColumnPr mapId="3" xpath="/Info/InfoLine/short_info" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E3A38290-2CCF-43BF-8714-B53ABE4F6506}" uniqueName="opens" name="opens" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{E3A38290-2CCF-43BF-8714-B53ABE4F6506}" uniqueName="opens" name="opens" dataDxfId="3">
       <xmlColumnPr mapId="3" xpath="/Info/InfoLine/opens" xmlDataType="time"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{508FBB80-CE31-427E-A301-A02524C3A11A}" uniqueName="closes" name="closes" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{508FBB80-CE31-427E-A301-A02524C3A11A}" uniqueName="closes" name="closes" dataDxfId="2">
       <xmlColumnPr mapId="3" xpath="/Info/InfoLine/closes" xmlDataType="time"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{974B90A1-BFCB-49AD-AB3E-FCC676FD751C}" uniqueName="full_info" name="full_info">
+    <tableColumn id="7" xr3:uid="{974B90A1-BFCB-49AD-AB3E-FCC676FD751C}" uniqueName="full_info" name="full_info" dataDxfId="1">
       <xmlColumnPr mapId="3" xpath="/Info/InfoLine/full_info" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -542,94 +797,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7220D0B-5AD5-4224-9620-517B81654667}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="11.85546875" customWidth="1"/>
+    <col min="5" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="119.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="P4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="P5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.37847222222222227</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.79513888888888884</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.37847222222222227</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.79513888888888884</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="P8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="P9" s="4"/>
+    </row>
+    <row r="10" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="P10" s="4"/>
+    </row>
+    <row r="11" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="P11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="P12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="P13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="P14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="8">
+        <v>0.375</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G15" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>